<commit_message>
Added results from sailsim to excel doc for interpol
</commit_message>
<xml_diff>
--- a/sim/liftdrag.xlsx
+++ b/sim/liftdrag.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\fzuend\Documents\Projekte\WindCommander\sim\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="22035" windowHeight="11055"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>lift</t>
   </si>
@@ -34,6 +39,39 @@
   </si>
   <si>
     <t>max geschw</t>
+  </si>
+  <si>
+    <t>dritte methode: gesampled von sailsim</t>
+  </si>
+  <si>
+    <t>heading</t>
+  </si>
+  <si>
+    <t>heel degree</t>
+  </si>
+  <si>
+    <t>max speed kn</t>
+  </si>
+  <si>
+    <t>in in irons</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>leeway</t>
+  </si>
+  <si>
+    <t>6kn wind von 0 grad aus</t>
+  </si>
+  <si>
+    <t>15kn wind  von 0 grad aus</t>
+  </si>
+  <si>
+    <t>30kn wind  von 0 grad aus</t>
+  </si>
+  <si>
+    <t>segel winkel geschätzt</t>
   </si>
 </sst>
 </file>
@@ -73,13 +111,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -88,7 +129,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -362,13 +403,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39423360"/>
-        <c:axId val="39244928"/>
+        <c:axId val="217570112"/>
+        <c:axId val="217571288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39423360"/>
+        <c:axId val="217570112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -378,7 +418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39244928"/>
+        <c:crossAx val="217571288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -386,7 +426,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39244928"/>
+        <c:axId val="217571288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -397,7 +437,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39423360"/>
+        <c:crossAx val="217570112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -422,7 +462,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -510,13 +550,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="46435712"/>
-        <c:axId val="46437504"/>
+        <c:axId val="217565408"/>
+        <c:axId val="217564624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="46435712"/>
+        <c:axId val="217565408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +565,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46437504"/>
+        <c:crossAx val="217564624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -534,7 +573,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46437504"/>
+        <c:axId val="217564624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -545,7 +584,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46435712"/>
+        <c:crossAx val="217565408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -751,7 +790,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -786,7 +825,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -995,15 +1034,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D28"/>
+  <dimension ref="A3:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1207,9 +1249,659 @@
         <v>0.6</v>
       </c>
     </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>360</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>345</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>340</v>
+      </c>
+      <c r="B44">
+        <v>0.9</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>320</v>
+      </c>
+      <c r="B45">
+        <v>2.1</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="F45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>308</v>
+      </c>
+      <c r="B46">
+        <v>2.6</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>290</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>284</v>
+      </c>
+      <c r="B48">
+        <v>2.9</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>270</v>
+      </c>
+      <c r="B49">
+        <v>2.9</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>250</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>238</v>
+      </c>
+      <c r="B51">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>222</v>
+      </c>
+      <c r="B52">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>208</v>
+      </c>
+      <c r="B53">
+        <v>1.9</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>193</v>
+      </c>
+      <c r="B54">
+        <v>1.8</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>180</v>
+      </c>
+      <c r="B55">
+        <v>1.8</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>360</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>330</v>
+      </c>
+      <c r="B64">
+        <v>3.4</v>
+      </c>
+      <c r="C64">
+        <v>11</v>
+      </c>
+      <c r="D64">
+        <v>4</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>318</v>
+      </c>
+      <c r="B65">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C65">
+        <v>13</v>
+      </c>
+      <c r="D65">
+        <v>4</v>
+      </c>
+      <c r="F65">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>309</v>
+      </c>
+      <c r="B66">
+        <v>5.6</v>
+      </c>
+      <c r="C66">
+        <v>14</v>
+      </c>
+      <c r="D66">
+        <v>4</v>
+      </c>
+      <c r="F66">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>286</v>
+      </c>
+      <c r="B67">
+        <v>6.1</v>
+      </c>
+      <c r="C67">
+        <v>12</v>
+      </c>
+      <c r="D67">
+        <v>3</v>
+      </c>
+      <c r="F67">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>268</v>
+      </c>
+      <c r="B68">
+        <v>6.4</v>
+      </c>
+      <c r="C68">
+        <v>8</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="F68">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>247</v>
+      </c>
+      <c r="B69">
+        <v>6.7</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="F69">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>238</v>
+      </c>
+      <c r="B70">
+        <v>5.9</v>
+      </c>
+      <c r="C70">
+        <v>3</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="F70">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>214</v>
+      </c>
+      <c r="B71">
+        <v>5.2</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>180</v>
+      </c>
+      <c r="B72">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>7</v>
+      </c>
+      <c r="B78" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>360</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>329</v>
+      </c>
+      <c r="B80">
+        <v>3.8</v>
+      </c>
+      <c r="C80">
+        <v>38</v>
+      </c>
+      <c r="D80">
+        <v>4</v>
+      </c>
+      <c r="F80">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>316</v>
+      </c>
+      <c r="B81">
+        <v>3.7</v>
+      </c>
+      <c r="C81">
+        <v>40</v>
+      </c>
+      <c r="D81">
+        <v>3</v>
+      </c>
+      <c r="F81">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>300</v>
+      </c>
+      <c r="B82">
+        <v>3.9</v>
+      </c>
+      <c r="C82">
+        <v>40</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
+      </c>
+      <c r="F82">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>279</v>
+      </c>
+      <c r="B83">
+        <v>4.5</v>
+      </c>
+      <c r="C83">
+        <v>32</v>
+      </c>
+      <c r="D83">
+        <v>3</v>
+      </c>
+      <c r="F83">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>262</v>
+      </c>
+      <c r="B84">
+        <v>5.4</v>
+      </c>
+      <c r="C84">
+        <v>21</v>
+      </c>
+      <c r="D84">
+        <v>2</v>
+      </c>
+      <c r="F84">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>250</v>
+      </c>
+      <c r="B85">
+        <v>6</v>
+      </c>
+      <c r="C85">
+        <v>13</v>
+      </c>
+      <c r="D85">
+        <v>2</v>
+      </c>
+      <c r="F85">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>220</v>
+      </c>
+      <c r="B86">
+        <v>6.3</v>
+      </c>
+      <c r="C86">
+        <v>3</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>200</v>
+      </c>
+      <c r="B87">
+        <v>6.1</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>180</v>
+      </c>
+      <c r="B88">
+        <v>6.1</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1219,7 +1911,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1231,7 +1923,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added also samples of sail angle
</commit_message>
<xml_diff>
--- a/sim/liftdrag.xlsx
+++ b/sim/liftdrag.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\fzuend\Documents\Projekte\WindCommander\sim\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="22035" windowHeight="11055"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="29">
   <si>
     <t>lift</t>
   </si>
@@ -72,6 +67,42 @@
   </si>
   <si>
     <t>segel winkel geschätzt</t>
+  </si>
+  <si>
+    <t>Segel pos sampling</t>
+  </si>
+  <si>
+    <t>heading 45</t>
+  </si>
+  <si>
+    <t>segel</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heel </t>
+  </si>
+  <si>
+    <t>wind 15kn</t>
+  </si>
+  <si>
+    <t>wind 0deg</t>
+  </si>
+  <si>
+    <t>in irons</t>
+  </si>
+  <si>
+    <t>heading 90deg</t>
+  </si>
+  <si>
+    <t>heading 135deg</t>
+  </si>
+  <si>
+    <t>headgin 180deg</t>
+  </si>
+  <si>
+    <t>alt heading</t>
   </si>
 </sst>
 </file>
@@ -111,7 +142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -129,7 +160,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -193,7 +224,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$13</c:f>
+              <c:f>Sheet1!$C$5:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -276,7 +307,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$13</c:f>
+              <c:f>Sheet1!$D$5:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -359,7 +390,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$13</c:f>
+              <c:f>Sheet1!$E$5:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -403,12 +434,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="217570112"/>
-        <c:axId val="217571288"/>
+        <c:axId val="123564800"/>
+        <c:axId val="123566336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="217570112"/>
+        <c:axId val="123564800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -418,7 +450,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217571288"/>
+        <c:crossAx val="123566336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -426,7 +458,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217571288"/>
+        <c:axId val="123566336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -437,7 +469,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217570112"/>
+        <c:crossAx val="123564800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -462,7 +494,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -518,7 +550,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$24:$B$28</c:f>
+              <c:f>Sheet1!$C$24:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -550,12 +582,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="217565408"/>
-        <c:axId val="217564624"/>
+        <c:axId val="123590912"/>
+        <c:axId val="123592704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="217565408"/>
+        <c:axId val="123590912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -565,7 +598,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217564624"/>
+        <c:crossAx val="123592704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -573,7 +606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217564624"/>
+        <c:axId val="123592704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -584,7 +617,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217565408"/>
+        <c:crossAx val="123590912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -610,13 +643,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>319087</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>14287</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
@@ -640,13 +673,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>427235</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>10635</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>151248</xdr:rowOff>
@@ -678,13 +711,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>328612</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -708,13 +741,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>133129</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>125001</xdr:rowOff>
@@ -790,7 +823,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -825,7 +858,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1034,868 +1067,1325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F88"/>
+  <dimension ref="A3:G135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <f>C5+B5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>D5+C5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.8</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.4</v>
       </c>
-      <c r="D6">
-        <f t="shared" ref="D6:D13" si="0">C6+B6</f>
+      <c r="E6">
+        <f t="shared" ref="E6:E13" si="0">D6+C6</f>
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>1.4</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.7</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>2.0999999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>40</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
       <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>2.15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>50</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>1.2</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
       <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>60</v>
       </c>
-      <c r="B10">
-        <v>0.9</v>
-      </c>
       <c r="C10">
         <v>0.9</v>
       </c>
       <c r="D10">
+        <v>0.9</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>70</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>0.6</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
       <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>80</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>0.3</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <f t="shared" si="0"/>
         <v>1.4000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>90</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
       <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
         <v>1.3</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>-0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>45</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>0.4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>90</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>0.9</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>135</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>180</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>0.6</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>7</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>9</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>8</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>12</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>10</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>360</v>
       </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
       <c r="C42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
         <v>11</v>
       </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>345</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
       <c r="C43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
         <v>11</v>
       </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>340</v>
       </c>
-      <c r="B44">
+      <c r="C44">
         <v>0.9</v>
       </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
       <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
         <v>4</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>320</v>
       </c>
-      <c r="B45">
+      <c r="C45">
         <v>2.1</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>2</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>4</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>308</v>
       </c>
-      <c r="B46">
+      <c r="C46">
         <v>2.6</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <v>2</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>290</v>
       </c>
-      <c r="B47">
+      <c r="C47">
         <v>3</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>2</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>3</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>284</v>
       </c>
-      <c r="B48">
+      <c r="C48">
         <v>2.9</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <v>2</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>270</v>
       </c>
-      <c r="B49">
+      <c r="C49">
         <v>2.9</v>
       </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
       <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>250</v>
       </c>
-      <c r="B50">
+      <c r="C50">
         <v>3</v>
       </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
       <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>238</v>
       </c>
-      <c r="B51">
+      <c r="C51">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C51">
-        <v>0</v>
-      </c>
       <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
         <v>2</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>222</v>
       </c>
-      <c r="B52">
+      <c r="C52">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
       <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>208</v>
       </c>
-      <c r="B53">
+      <c r="C53">
         <v>1.9</v>
       </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
       <c r="D53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>193</v>
       </c>
-      <c r="B54">
+      <c r="C54">
         <v>1.8</v>
       </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
       <c r="D54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>180</v>
       </c>
-      <c r="B55">
+      <c r="C55">
         <v>1.8</v>
       </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
       <c r="D55">
         <v>0</v>
       </c>
-      <c r="F55">
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="G55">
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>7</v>
       </c>
       <c r="B62" t="s">
+        <v>28</v>
+      </c>
+      <c r="C62" t="s">
         <v>9</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>8</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>12</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>10</v>
       </c>
-      <c r="F62" t="s">
+      <c r="G62" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>360</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <f>A63-180</f>
+        <v>180</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63">
-        <v>0</v>
-      </c>
-      <c r="E63" t="s">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63" t="s">
         <v>11</v>
       </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>330</v>
       </c>
       <c r="B64">
+        <f t="shared" ref="B64:B72" si="1">A64-180</f>
+        <v>150</v>
+      </c>
+      <c r="C64">
         <v>3.4</v>
       </c>
-      <c r="C64">
+      <c r="D64">
         <v>11</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <v>4</v>
       </c>
-      <c r="F64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>318</v>
       </c>
       <c r="B65">
+        <f t="shared" si="1"/>
+        <v>138</v>
+      </c>
+      <c r="C65">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C65">
+      <c r="D65">
         <v>13</v>
       </c>
-      <c r="D65">
+      <c r="E65">
         <v>4</v>
       </c>
-      <c r="F65">
+      <c r="G65">
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>309</v>
       </c>
       <c r="B66">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="C66">
         <v>5.6</v>
       </c>
-      <c r="C66">
+      <c r="D66">
         <v>14</v>
       </c>
-      <c r="D66">
+      <c r="E66">
         <v>4</v>
       </c>
-      <c r="F66">
+      <c r="G66">
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>286</v>
       </c>
       <c r="B67">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="C67">
         <v>6.1</v>
       </c>
-      <c r="C67">
+      <c r="D67">
         <v>12</v>
       </c>
-      <c r="D67">
+      <c r="E67">
         <v>3</v>
       </c>
-      <c r="F67">
+      <c r="G67">
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>268</v>
       </c>
       <c r="B68">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="C68">
         <v>6.4</v>
       </c>
-      <c r="C68">
+      <c r="D68">
         <v>8</v>
       </c>
-      <c r="D68">
+      <c r="E68">
         <v>3</v>
       </c>
-      <c r="F68">
+      <c r="G68">
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>247</v>
       </c>
       <c r="B69">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="C69">
         <v>6.7</v>
       </c>
-      <c r="C69">
+      <c r="D69">
         <v>4</v>
       </c>
-      <c r="D69">
+      <c r="E69">
         <v>2</v>
       </c>
-      <c r="F69">
+      <c r="G69">
         <v>41</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>238</v>
       </c>
       <c r="B70">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="C70">
         <v>5.9</v>
       </c>
-      <c r="C70">
+      <c r="D70">
         <v>3</v>
       </c>
-      <c r="D70">
+      <c r="E70">
         <v>2</v>
       </c>
-      <c r="F70">
+      <c r="G70">
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>214</v>
       </c>
       <c r="B71">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="C71">
         <v>5.2</v>
       </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
       <c r="D71">
         <v>1</v>
       </c>
-      <c r="F71">
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="G71">
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>180</v>
       </c>
       <c r="B72">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C72">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
       <c r="D72">
         <v>0</v>
       </c>
-      <c r="F72">
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="G72">
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>7</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>9</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>8</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>12</v>
       </c>
-      <c r="E78" t="s">
+      <c r="F78" t="s">
         <v>10</v>
       </c>
-      <c r="F78" t="s">
+      <c r="G78" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>360</v>
       </c>
-      <c r="B79">
-        <v>0</v>
-      </c>
       <c r="C79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79">
-        <v>0</v>
-      </c>
-      <c r="E79" t="s">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79" t="s">
         <v>11</v>
       </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>329</v>
       </c>
-      <c r="B80">
+      <c r="C80">
         <v>3.8</v>
       </c>
-      <c r="C80">
+      <c r="D80">
         <v>38</v>
       </c>
-      <c r="D80">
+      <c r="E80">
         <v>4</v>
       </c>
-      <c r="F80">
+      <c r="G80">
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>316</v>
       </c>
-      <c r="B81">
+      <c r="C81">
         <v>3.7</v>
       </c>
-      <c r="C81">
+      <c r="D81">
         <v>40</v>
       </c>
-      <c r="D81">
+      <c r="E81">
         <v>3</v>
       </c>
-      <c r="F81">
+      <c r="G81">
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>300</v>
       </c>
-      <c r="B82">
+      <c r="C82">
         <v>3.9</v>
       </c>
-      <c r="C82">
+      <c r="D82">
         <v>40</v>
       </c>
-      <c r="D82">
+      <c r="E82">
         <v>3</v>
       </c>
-      <c r="F82">
+      <c r="G82">
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>279</v>
       </c>
-      <c r="B83">
+      <c r="C83">
         <v>4.5</v>
       </c>
-      <c r="C83">
+      <c r="D83">
         <v>32</v>
       </c>
-      <c r="D83">
+      <c r="E83">
         <v>3</v>
       </c>
-      <c r="F83">
+      <c r="G83">
         <v>35</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>262</v>
       </c>
-      <c r="B84">
+      <c r="C84">
         <v>5.4</v>
       </c>
-      <c r="C84">
+      <c r="D84">
         <v>21</v>
       </c>
-      <c r="D84">
+      <c r="E84">
         <v>2</v>
       </c>
-      <c r="F84">
+      <c r="G84">
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>250</v>
       </c>
-      <c r="B85">
+      <c r="C85">
         <v>6</v>
       </c>
-      <c r="C85">
+      <c r="D85">
         <v>13</v>
       </c>
-      <c r="D85">
+      <c r="E85">
         <v>2</v>
       </c>
-      <c r="F85">
+      <c r="G85">
         <v>45</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>220</v>
       </c>
-      <c r="B86">
+      <c r="C86">
         <v>6.3</v>
       </c>
-      <c r="C86">
+      <c r="D86">
         <v>3</v>
       </c>
-      <c r="D86">
-        <v>1</v>
-      </c>
-      <c r="F86">
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="G86">
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>200</v>
       </c>
-      <c r="B87">
+      <c r="C87">
         <v>6.1</v>
       </c>
-      <c r="C87">
-        <v>1</v>
-      </c>
       <c r="D87">
         <v>1</v>
       </c>
-      <c r="F87">
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="G87">
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>180</v>
       </c>
-      <c r="B88">
+      <c r="C88">
         <v>6.1</v>
       </c>
-      <c r="C88">
-        <v>0</v>
-      </c>
       <c r="D88">
         <v>0</v>
       </c>
-      <c r="F88">
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="G88">
         <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>19</v>
+      </c>
+      <c r="C97" t="s">
+        <v>20</v>
+      </c>
+      <c r="D97" t="s">
+        <v>21</v>
+      </c>
+      <c r="E97" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>3.6</v>
+      </c>
+      <c r="D98">
+        <v>10</v>
+      </c>
+      <c r="E98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>20</v>
+      </c>
+      <c r="C99">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D99">
+        <v>8</v>
+      </c>
+      <c r="E99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>40</v>
+      </c>
+      <c r="C100">
+        <v>4</v>
+      </c>
+      <c r="D100">
+        <v>7</v>
+      </c>
+      <c r="E100">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>19</v>
+      </c>
+      <c r="C106" t="s">
+        <v>20</v>
+      </c>
+      <c r="D106" t="s">
+        <v>21</v>
+      </c>
+      <c r="E106" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>0</v>
+      </c>
+      <c r="C107">
+        <v>3.7</v>
+      </c>
+      <c r="D107">
+        <v>9</v>
+      </c>
+      <c r="E107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>10</v>
+      </c>
+      <c r="C108">
+        <v>3.9</v>
+      </c>
+      <c r="D108">
+        <v>10</v>
+      </c>
+      <c r="E108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>25</v>
+      </c>
+      <c r="C109">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D109">
+        <v>9</v>
+      </c>
+      <c r="E109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>30</v>
+      </c>
+      <c r="C110">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D110">
+        <v>8</v>
+      </c>
+      <c r="E110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>45</v>
+      </c>
+      <c r="C111">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D111">
+        <v>7</v>
+      </c>
+      <c r="E111">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>55</v>
+      </c>
+      <c r="C112">
+        <v>4.8</v>
+      </c>
+      <c r="D112">
+        <v>6</v>
+      </c>
+      <c r="E112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>70</v>
+      </c>
+      <c r="C113">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D113">
+        <v>5</v>
+      </c>
+      <c r="E113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>19</v>
+      </c>
+      <c r="C118" t="s">
+        <v>20</v>
+      </c>
+      <c r="D118" t="s">
+        <v>21</v>
+      </c>
+      <c r="E118" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>0</v>
+      </c>
+      <c r="C119">
+        <v>1.8</v>
+      </c>
+      <c r="D119">
+        <v>2</v>
+      </c>
+      <c r="E119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>10</v>
+      </c>
+      <c r="C120">
+        <v>3.3</v>
+      </c>
+      <c r="D120">
+        <v>2</v>
+      </c>
+      <c r="E120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>20</v>
+      </c>
+      <c r="C121">
+        <v>3.6</v>
+      </c>
+      <c r="D121">
+        <v>2</v>
+      </c>
+      <c r="E121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>30</v>
+      </c>
+      <c r="C122">
+        <v>3.8</v>
+      </c>
+      <c r="D122">
+        <v>2</v>
+      </c>
+      <c r="E122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>45</v>
+      </c>
+      <c r="C123">
+        <v>4.3</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>60</v>
+      </c>
+      <c r="C124">
+        <v>4.7</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>90</v>
+      </c>
+      <c r="C125">
+        <v>4</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+      <c r="E125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>19</v>
+      </c>
+      <c r="C129" t="s">
+        <v>20</v>
+      </c>
+      <c r="D129" t="s">
+        <v>21</v>
+      </c>
+      <c r="E129" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>25</v>
+      </c>
+      <c r="C131">
+        <v>2.6</v>
+      </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>45</v>
+      </c>
+      <c r="C132">
+        <v>2.9</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>60</v>
+      </c>
+      <c r="C133">
+        <v>3.3</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>70</v>
+      </c>
+      <c r="C134">
+        <v>3.6</v>
+      </c>
+      <c r="D134">
+        <v>0</v>
+      </c>
+      <c r="E134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>90</v>
+      </c>
+      <c r="C135">
+        <v>3.9</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1911,7 +2401,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1923,7 +2413,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>